<commit_message>
after prototype 0.7.4 - final 0.8
</commit_message>
<xml_diff>
--- a/codm-wifi-pixel-controller.bom.xlsx
+++ b/codm-wifi-pixel-controller.bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pm/Nextcloud/eagle/projects/neopixel/wled-controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD5DC8-062E-984A-A8A8-FDF457DEAA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEDC627-0D4D-3540-8053-4B4262BC2E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31140" yWindow="2980" windowWidth="27640" windowHeight="16860" xr2:uid="{3BAFE283-D07F-EC4D-8CA8-63E97A4C28F7}"/>
+    <workbookView xWindow="5180" yWindow="3040" windowWidth="28040" windowHeight="17360" xr2:uid="{7E72A688-2485-DF4A-9118-D153189F0A91}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>Qty</t>
   </si>
@@ -60,55 +60,106 @@
     <t>WS-TASV J-Bend SMT Tact Switch 3.5x2.9 mm</t>
   </si>
   <si>
-    <t>LEDCHIPLED_0805</t>
-  </si>
-  <si>
-    <t>CHIPLED_0805</t>
-  </si>
-  <si>
-    <t>STATUS</t>
+    <t>PINHD-1X5</t>
+  </si>
+  <si>
+    <t>1X05</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>PIN HEADER</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>C-EUC0603K</t>
+  </si>
+  <si>
+    <t>C0603K</t>
+  </si>
+  <si>
+    <t>CAPACITOR, European symbol</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R-EU_R0603</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>RESISTOR, European symbol</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>C-EUC0805K</t>
+  </si>
+  <si>
+    <t>C0805K</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>150080RS75000</t>
+  </si>
+  <si>
+    <t>LEDCHIP-LED0805</t>
+  </si>
+  <si>
+    <t>CHIP-LED0805</t>
   </si>
   <si>
     <t>LED</t>
   </si>
   <si>
-    <t>PINHD-1X5</t>
-  </si>
-  <si>
-    <t>1X05</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
-  </si>
-  <si>
-    <t>SJ</t>
-  </si>
-  <si>
-    <t>EN-2ND</t>
-  </si>
-  <si>
-    <t>SMD solder JUMPER</t>
-  </si>
-  <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>C-EUC0603K</t>
-  </si>
-  <si>
-    <t>C0603K</t>
-  </si>
-  <si>
-    <t>C1, C3, C6, C10</t>
-  </si>
-  <si>
-    <t>CAPACITOR, European symbol</t>
-  </si>
-  <si>
-    <t>10k</t>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>22k1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>22uF/6.3V/20%</t>
+  </si>
+  <si>
+    <t>C4, C7</t>
+  </si>
+  <si>
+    <t>2k7</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>3.3uH</t>
+  </si>
+  <si>
+    <t>WE-LQ_1812_744045003</t>
+  </si>
+  <si>
+    <t>WE-LQ_1812</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>WE-LQ SMD Inductor</t>
   </si>
   <si>
     <t>4R-NEXB38V</t>
@@ -123,43 +174,16 @@
     <t>Array Chip Resistor</t>
   </si>
   <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>C-EUC0805</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>10uF/25V</t>
-  </si>
-  <si>
-    <t>C-EUC0805K</t>
-  </si>
-  <si>
-    <t>C0805K</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>10µ</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>C7, C8, C9</t>
-  </si>
-  <si>
-    <t>24V 500mA (507-1803-1-ND)</t>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>WS-TASV SMT Tact Switch 6x6 mm</t>
+  </si>
+  <si>
+    <t>69k8</t>
+  </si>
+  <si>
+    <t>R1</t>
   </si>
   <si>
     <t>PTCFUSE-1206</t>
@@ -174,34 +198,16 @@
     <t>PTC fuses, resettable thermistors</t>
   </si>
   <si>
-    <t>2k7</t>
-  </si>
-  <si>
-    <t>R-EU_R0603</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RESISTOR, European symbol</t>
-  </si>
-  <si>
-    <t>R1, R3</t>
-  </si>
-  <si>
-    <t>ESP-WROOM-02</t>
-  </si>
-  <si>
-    <t>MODULE_ESP-WROOM-02</t>
+    <t>AP62XXX-TSOT26</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>Wi-Fi Module w/ESP8266 802.11b/g/n 20dBm 20x18x3mm</t>
+    <t>ESP-WROOM-32</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
   <si>
     <t>MCV-1,5/4-G-3,81</t>
@@ -210,25 +216,13 @@
     <t>U$101</t>
   </si>
   <si>
-    <t>PTR1TP14R</t>
-  </si>
-  <si>
-    <t>TP14R</t>
-  </si>
-  <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9</t>
-  </si>
-  <si>
-    <t>TEST PIN</t>
-  </si>
-  <si>
     <t>REG710NA-5/250</t>
   </si>
   <si>
     <t>SOT95P280X145-6N</t>
   </si>
   <si>
-    <t>U4</t>
+    <t>U2</t>
   </si>
   <si>
     <t>Check prices</t>
@@ -249,28 +243,31 @@
     <t>DIODE</t>
   </si>
   <si>
-    <t>SN74AHCT125D</t>
-  </si>
-  <si>
-    <t>SOIC127P600X175-14N</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
-    <t>TLV1117LV33DCYR</t>
-  </si>
-  <si>
-    <t>VREG_TLV1117LV33DCYR</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>1-A, low-dropout voltage regulator 4-SOT-223 -40 to 125  Check prices</t>
-  </si>
-  <si>
-    <t>wifi pixel controller 0.7.2</t>
+    <t>24V 500mA</t>
+  </si>
+  <si>
+    <t>SN74AHCT125PWR</t>
+  </si>
+  <si>
+    <t>SOP65P640X120-14N</t>
+  </si>
+  <si>
+    <t>Check availability</t>
+  </si>
+  <si>
+    <t>WLED Controller V0.8</t>
+  </si>
+  <si>
+    <t>C2, C3, C6, C11</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>C8, C9, C10</t>
   </si>
 </sst>
 </file>
@@ -302,7 +299,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -310,56 +307,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -380,17 +334,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CE6FB2C-65BA-5345-ACF2-2857B6F8DC23}" name="Tabelle1" displayName="Tabelle1" ref="B3:G23" totalsRowShown="0">
-  <autoFilter ref="B3:G23" xr:uid="{8CE6FB2C-65BA-5345-ACF2-2857B6F8DC23}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{676E9A73-0DFB-DE43-8996-F4203D1D120F}" name="Tabelle1" displayName="Tabelle1" ref="B3:G25" totalsRowShown="0">
+  <autoFilter ref="B3:G25" xr:uid="{676E9A73-0DFB-DE43-8996-F4203D1D120F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{98F3D4A5-B2D0-F448-B8D0-442AD570A045}" name="Qty"/>
-    <tableColumn id="2" xr3:uid="{0C61AF80-0A2A-9C47-BB93-50F6AC6E66DD}" name="Value"/>
-    <tableColumn id="3" xr3:uid="{1A6A3C6F-F5B4-FD44-89FC-943F36BE6815}" name="Device"/>
-    <tableColumn id="4" xr3:uid="{8F0BF06E-E7BE-994B-8845-F8F007098E9D}" name="Package"/>
-    <tableColumn id="5" xr3:uid="{B1089286-DFEC-6A4B-ADC3-81908B637DCF}" name="Parts"/>
-    <tableColumn id="6" xr3:uid="{56866249-56F7-4F49-A195-03EB514A5BD7}" name="Description"/>
+    <tableColumn id="1" xr3:uid="{4FC9B8EE-7628-544D-9149-BFBE986BC0EE}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{22BB1A9A-3945-A44F-82C7-05FF668C9BFC}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{7029F8FE-4582-AF4D-B0C3-9A82F40F3306}" name="Device"/>
+    <tableColumn id="4" xr3:uid="{E700B0A6-014D-1143-A39A-EAE952F10D00}" name="Package"/>
+    <tableColumn id="5" xr3:uid="{41D309C7-A595-EB41-8320-F0C374711D38}" name="Parts"/>
+    <tableColumn id="6" xr3:uid="{12C2D923-EA2C-DD46-B926-9AB72B6A6D04}" name="Description"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -690,58 +644,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17E397C-D168-0F44-BFAA-E496BC39C4C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E82323B-520B-FB4C-9A1D-D9F46BF4EDF0}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G23"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="69.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="60.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" ht="31" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -799,16 +757,19 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
@@ -816,39 +777,42 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -868,7 +832,7 @@
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
@@ -876,39 +840,39 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -916,39 +880,39 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
@@ -956,19 +920,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
@@ -976,96 +940,99 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>330</v>
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>52</v>
+      <c r="C17">
+        <v>330</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>56</v>
+      <c r="C18">
+        <v>430182070816</v>
+      </c>
+      <c r="D18">
+        <v>430182070816</v>
+      </c>
+      <c r="E18">
+        <v>430182070816</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
@@ -1073,19 +1040,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -1093,19 +1057,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -1113,19 +1074,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -1133,19 +1091,59 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1153,7 +1151,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>